<commit_message>
Competing risk event survival analysis
</commit_message>
<xml_diff>
--- a/Figures_Tables/result_tables/tables.xlsx
+++ b/Figures_Tables/result_tables/tables.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="13880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="13840" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
     <sheet name="Sensitivity study" sheetId="3" r:id="rId3"/>
     <sheet name="Ps model" sheetId="4" r:id="rId4"/>
+    <sheet name="Table2_New" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="130000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="244">
+  <si>
+    <t>Discharge from ICU</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discharge from Hospital</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extubation</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.61~0.86</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6~0.84</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.63~0.87</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
   <si>
     <t>-1.28 (-1.44~-1.11)</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -76,6 +101,18 @@
   <si>
     <t>Ventilation time
 (non-surviors)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Secondary Outcome</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subhazard Ratio</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>95% CI</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -1070,7 +1107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1134,6 +1171,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1168,6 +1208,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1519,15 +1574,15 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
@@ -1535,65 +1590,65 @@
     <row r="2" spans="1:7" ht="17" customHeight="1" thickBot="1">
       <c r="A2" s="13"/>
       <c r="B2" s="15" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" customHeight="1" thickTop="1">
       <c r="A3" s="11" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="D4" s="17">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="G4" s="18">
         <v>0.4</v>
@@ -1601,22 +1656,22 @@
     </row>
     <row r="5" spans="1:7" ht="25" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="D5" s="18">
         <v>0.36</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="G5" s="18">
         <v>0.36</v>
@@ -1624,22 +1679,22 @@
     </row>
     <row r="6" spans="1:7" ht="17" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G6" s="18">
         <v>0.6</v>
@@ -1647,12 +1702,12 @@
     </row>
     <row r="7" spans="1:7" ht="17" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
       <c r="D7" s="22" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
@@ -1662,45 +1717,45 @@
     </row>
     <row r="8" spans="1:7" ht="17" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>79</v>
+        <v>87</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>88</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="18" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:7" ht="17" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="18" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:7" ht="24" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -1711,22 +1766,22 @@
     </row>
     <row r="11" spans="1:7" ht="17" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D11" s="18">
         <v>0.7</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="G11" s="18">
         <v>0.4</v>
@@ -1734,22 +1789,22 @@
     </row>
     <row r="12" spans="1:7" ht="17" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D12" s="18">
         <v>0.1</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G12" s="18">
         <v>0.7</v>
@@ -1757,22 +1812,22 @@
     </row>
     <row r="13" spans="1:7" ht="17" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D13" s="18">
         <v>0.8</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="G13" s="18">
         <v>0.7</v>
@@ -1780,22 +1835,22 @@
     </row>
     <row r="14" spans="1:7" ht="17" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D14" s="18">
         <v>0.2</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G14" s="18">
         <v>0.6</v>
@@ -1803,22 +1858,22 @@
     </row>
     <row r="15" spans="1:7" ht="17" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D15" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="G15" s="18">
         <v>0.5</v>
@@ -1826,22 +1881,22 @@
     </row>
     <row r="16" spans="1:7" ht="17" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D16" s="18">
         <v>0.5</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="G16" s="18">
         <v>0.8</v>
@@ -1849,22 +1904,22 @@
     </row>
     <row r="17" spans="1:7" ht="17" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D17" s="17">
         <v>1E-4</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="G17" s="18">
         <v>1</v>
@@ -1872,22 +1927,22 @@
     </row>
     <row r="18" spans="1:7" ht="17" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D18" s="17">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="G18" s="18">
         <v>0.6</v>
@@ -1895,22 +1950,22 @@
     </row>
     <row r="19" spans="1:7" ht="26" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D19" s="17">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G19" s="18">
         <v>0.8</v>
@@ -1918,7 +1973,7 @@
     </row>
     <row r="20" spans="1:7" ht="17" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -1929,22 +1984,22 @@
     </row>
     <row r="21" spans="1:7" ht="17" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="G21" s="18">
         <v>0.3</v>
@@ -1952,22 +2007,22 @@
     </row>
     <row r="22" spans="1:7" ht="17" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="D22" s="17">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="G22" s="18">
         <v>0.5</v>
@@ -1975,22 +2030,22 @@
     </row>
     <row r="23" spans="1:7" ht="17" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="D23" s="18">
         <v>0.01</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="G23" s="18">
         <v>0.7</v>
@@ -1998,22 +2053,22 @@
     </row>
     <row r="24" spans="1:7" ht="17" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="D24" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G24" s="18">
         <v>0.6</v>
@@ -2021,22 +2076,22 @@
     </row>
     <row r="25" spans="1:7" ht="17" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D25" s="18">
         <v>0.77</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="G25" s="18">
         <v>0.8</v>
@@ -2044,22 +2099,22 @@
     </row>
     <row r="26" spans="1:7" ht="17" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="D26" s="18">
         <v>0.05</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="G26" s="18">
         <v>0.6</v>
@@ -2067,22 +2122,22 @@
     </row>
     <row r="27" spans="1:7" ht="17" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D27" s="17">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G27" s="18">
         <v>1</v>
@@ -2090,22 +2145,22 @@
     </row>
     <row r="28" spans="1:7" ht="17" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="D28" s="17">
         <v>0.02</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="G28" s="18">
         <v>0.3</v>
@@ -2113,22 +2168,22 @@
     </row>
     <row r="29" spans="1:7" ht="17" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="D29" s="18">
         <v>0.6</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="G29" s="18">
         <v>7.0000000000000007E-2</v>
@@ -2136,22 +2191,22 @@
     </row>
     <row r="30" spans="1:7" ht="17" customHeight="1">
       <c r="A30" s="10" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D30" s="18">
         <v>0.5</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G30" s="18">
         <v>0.7</v>
@@ -2159,22 +2214,22 @@
     </row>
     <row r="31" spans="1:7" ht="17" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D31" s="17">
         <v>0.02</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="G31" s="18">
         <v>0.2</v>
@@ -2191,22 +2246,22 @@
     </row>
     <row r="33" spans="1:7" ht="27" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G33" s="18">
         <v>0.2</v>
@@ -2214,22 +2269,22 @@
     </row>
     <row r="34" spans="1:7" ht="38" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="G34" s="18">
         <v>1</v>
@@ -2259,194 +2314,194 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView view="pageLayout" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22" customHeight="1" thickBot="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="22" customHeight="1" thickTop="1">
+      <c r="A2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="32" t="s">
+      <c r="B2" s="34">
+        <v>0.152</v>
+      </c>
+      <c r="C2" s="34">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="31">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" customHeight="1">
+      <c r="A3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" ht="22" customHeight="1">
+      <c r="A4" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" customHeight="1">
+      <c r="A5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="29">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" customHeight="1">
+      <c r="A6" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29" customHeight="1">
+      <c r="A7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="29">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" customHeight="1">
+      <c r="A8" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" customHeight="1">
+      <c r="A9" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="29">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29" customHeight="1">
+      <c r="A10" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E10" s="29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29" customHeight="1">
+      <c r="A11" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="22" customHeight="1" thickTop="1">
-      <c r="A2" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="33">
-        <v>0.152</v>
-      </c>
-      <c r="C2" s="33">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="30">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29" customHeight="1">
-      <c r="A3" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="27"/>
-    </row>
-    <row r="4" spans="1:5" ht="22" customHeight="1">
-      <c r="A4" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" customHeight="1">
-      <c r="A5" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="28">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29" customHeight="1">
-      <c r="A6" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29" customHeight="1">
-      <c r="A7" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="28">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29" customHeight="1">
-      <c r="A8" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29" customHeight="1">
-      <c r="A9" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="28">
-        <v>2.9999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="29" customHeight="1">
-      <c r="A10" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="29" customHeight="1">
-      <c r="A11" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="28">
+      <c r="E11" s="29">
         <v>0.3</v>
       </c>
     </row>
@@ -2478,23 +2533,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2502,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C7">
         <v>693</v>
@@ -2510,7 +2565,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="C8">
         <v>85.56</v>
@@ -2524,7 +2579,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="C10">
         <v>117</v>
@@ -2532,7 +2587,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="5" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C11">
         <v>14.44</v>
@@ -2540,10 +2595,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C13">
         <v>810</v>
@@ -2551,7 +2606,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C14">
         <v>100</v>
@@ -2562,7 +2617,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C16" s="5">
         <v>0.42399999999999999</v>
@@ -2597,38 +2652,38 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="G3" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="B5" s="3">
         <v>0.99664870000000005</v>
@@ -2651,7 +2706,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B6" s="3">
         <v>1.000894</v>
@@ -2674,7 +2729,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B7" s="3">
         <v>1.59127</v>
@@ -2697,7 +2752,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="B8" s="3">
         <v>7.2156000000000002</v>
@@ -2726,7 +2781,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2735,7 +2790,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B11" s="3">
         <v>1.5041310000000001</v>
@@ -2758,7 +2813,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B12" s="3">
         <v>1.183298</v>
@@ -2781,7 +2836,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="B13" s="3">
         <v>1.5754729999999999</v>
@@ -2804,7 +2859,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B14" s="3">
         <v>1.4919450000000001</v>
@@ -2827,7 +2882,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B15" s="3">
         <v>1.9040029999999999</v>
@@ -2850,7 +2905,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B16" s="3">
         <v>1.127912</v>
@@ -2879,7 +2934,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B18" s="3">
         <v>1.0259119999999999</v>
@@ -2902,7 +2957,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B19" s="3">
         <v>1.7799700000000001</v>
@@ -2925,7 +2980,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="B20" s="3">
         <v>0.97763770000000005</v>
@@ -2948,7 +3003,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B21" s="3">
         <v>1.537355</v>
@@ -2971,7 +3026,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B22" s="3">
         <v>0.36014439999999998</v>
@@ -2994,7 +3049,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B23" s="3">
         <v>0.78372209999999998</v>
@@ -3017,7 +3072,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B24" s="3">
         <v>0.95840420000000004</v>
@@ -3040,7 +3095,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B25" s="3">
         <v>1.382242</v>
@@ -3063,7 +3118,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B26" s="3">
         <v>1.1597500000000001</v>
@@ -3086,7 +3141,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B27" s="3">
         <v>1.016337</v>
@@ -3109,7 +3164,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B28" s="3">
         <v>1.007226</v>
@@ -3132,7 +3187,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B29" s="3">
         <v>1.0063120000000001</v>
@@ -3155,7 +3210,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B30" s="3">
         <v>0.97394990000000004</v>
@@ -3178,7 +3233,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B31" s="3">
         <v>1.0002230000000001</v>
@@ -3201,7 +3256,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B32" s="3">
         <v>1.032224</v>
@@ -3224,7 +3279,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B33" s="3">
         <v>0.95359110000000002</v>
@@ -3247,7 +3302,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="B34" s="3">
         <v>0.99973749999999995</v>
@@ -3270,7 +3325,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="B35" s="4">
         <v>0.92980370000000001</v>
@@ -3293,7 +3348,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B36" s="4">
         <v>1.0222789999999999</v>
@@ -3316,7 +3371,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B37" s="4">
         <v>1.023301</v>
@@ -3339,7 +3394,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="B38" s="4">
         <v>1.055034</v>
@@ -3362,7 +3417,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="B39" s="4">
         <v>1.005822</v>
@@ -3385,7 +3440,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B40" s="4">
         <v>0.76309660000000001</v>
@@ -3408,7 +3463,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B41" s="4">
         <v>1.0007079999999999</v>
@@ -3431,7 +3486,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="B42" s="4">
         <v>0.99573080000000003</v>
@@ -3454,12 +3509,12 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3471,4 +3526,159 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="27" thickBot="1">
+      <c r="A1" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="27" thickTop="1">
+      <c r="A2" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="34">
+        <v>0.152</v>
+      </c>
+      <c r="C2" s="34">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="39">
+        <v>0.72</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="39">
+      <c r="A3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="41">
+        <v>0.71</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="39">
+      <c r="A4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="41">
+        <v>0.74</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="39">
+      <c r="A5" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="29"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Indication of MV comparison
</commit_message>
<xml_diff>
--- a/Figures_Tables/result_tables/tables.xlsx
+++ b/Figures_Tables/result_tables/tables.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="13960" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table 2_old" sheetId="2" r:id="rId2"/>
     <sheet name="Sensitivity study" sheetId="3" r:id="rId3"/>
     <sheet name="Ps model" sheetId="4" r:id="rId4"/>
     <sheet name="Table2_New" sheetId="5" r:id="rId5"/>
+    <sheet name="MV_indication_comparison" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="130000" concurrentCalc="0"/>
   <extLst>
@@ -23,651 +24,683 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="254">
+  <si>
+    <t>Pneumonia</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 (4.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 (5.4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>67 (20%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>68 (20.3%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>33 (4.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>70 (7.1%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>147 (18.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>152 (15.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>348 (50%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>51 (35~72)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>56 (40~73)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>53  (35~72)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>54 (38~73)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>aline_flg</t>
+  </si>
+  <si>
+    <t>Odds Ratio</t>
+  </si>
+  <si>
+    <t>Std. Err.</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>P&gt;z</t>
+  </si>
+  <si>
+    <t>[95% Conf.</t>
+  </si>
+  <si>
+    <t>Interval]</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>weight_first</t>
+  </si>
+  <si>
+    <t>sofa_first</t>
+  </si>
+  <si>
+    <t>hour_icu_intime</t>
+  </si>
+  <si>
+    <t>1.chf_flg</t>
+  </si>
+  <si>
+    <t>1.afib_flg</t>
+  </si>
+  <si>
+    <t>1.renal_flg</t>
+  </si>
+  <si>
+    <t>1.liver_flg</t>
+  </si>
+  <si>
+    <t>1.copd_flg</t>
+  </si>
+  <si>
+    <t>1.cad_flg</t>
+  </si>
+  <si>
+    <t>1.stroke_flg</t>
+  </si>
+  <si>
+    <t>1.mal_flg</t>
+  </si>
+  <si>
+    <t>1.resp_flg</t>
+  </si>
+  <si>
+    <t>map_1st</t>
+  </si>
+  <si>
+    <t>hr_1st</t>
+  </si>
+  <si>
+    <t>spo2_1st</t>
+  </si>
+  <si>
+    <t>temp_1st</t>
+  </si>
+  <si>
+    <t>wbc_first</t>
+  </si>
+  <si>
+    <t>hgb_first</t>
+  </si>
+  <si>
+    <t>platelet_first</t>
+  </si>
+  <si>
+    <t>sodium_first</t>
+  </si>
+  <si>
+    <t>potassium_first</t>
+  </si>
+  <si>
+    <t>tco2_first</t>
+  </si>
+  <si>
+    <t>chloride_first</t>
+  </si>
+  <si>
+    <t>bun_first</t>
+  </si>
+  <si>
+    <t>creatinine_first</t>
+  </si>
+  <si>
+    <t>po2_first</t>
+  </si>
+  <si>
+    <t>pco2_first</t>
+  </si>
+  <si>
+    <t>PS model</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>n=1491</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>day_icu_admission</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MICU (ref) vs CSRU</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mon</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tue</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wed</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thur</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fri</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sat</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUROC: 0.81</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HL: p=0.4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.8 (11.2 ~14.2)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.7 (8~14.8)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.5 (8.4~14.7)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>342        351</t>
+  </si>
+  <si>
+    <t>84.44      86.67</t>
+  </si>
+  <si>
+    <t>63         54</t>
+  </si>
+  <si>
+    <t>15.56      13.33</t>
+  </si>
+  <si>
+    <t>405        405</t>
+  </si>
+  <si>
+    <t>140 (138~143)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>140 (137~142)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>238 (184~303)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>238 (186~289)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>24 (22~27)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>24 (21~27)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 (3.6~4.5)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 (3.7~4.4)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 (11~22)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switched to DNR and CMO (redo)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>40 (35~46.5)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1075 (361~2385)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1299 (352~2743)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9 (0.5~1.3)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2 (1.4~3.2)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.75 (0.4~1.3)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1 (0.6~2.6)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 (1.4~2)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.7 (1.6~5.8)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 (2~7)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 (5~11)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 (2~7)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 (3~11)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;0.0001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.8 (1~2.8)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.8 (1.8~4.9)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1 (1.5~5)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.3 (2.3~7.3)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOFA Score</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHF</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARDS</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Renal Disease</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gender (Female)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>205 (58.9%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>192 (55.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 (4~6)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 (5~8)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;0.0001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 (4~7)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 (4~7)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Service Unit</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MICU</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>504 (63.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>290 (29.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>184 (52.9%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>192 (55.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SICU</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>288 (26.4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>164 (47.1%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>156 (44.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Co-morbidities</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>97 (12.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>116 (11.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>44 (12.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>36 (10.3%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>82 (10.4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>125 (12.7%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>32 (9.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>28 (3.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>32 (3.3%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>13 (3.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 (2.9%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>28 (4.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>61 (6.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>14 (4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 (5.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>81 (10.23%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>76 (7.72%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>39 (11.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>51 (6.4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>72 (7.32%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>23 (6.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>21 (6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>70 (8.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>152 (15.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>33 (9.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>92 (11.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>164 (16.7%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>51 (14.7%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>278 (35.1%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>287 (29.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>121 (34.7%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>125 (35.9%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.6 (7.8~14.3)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.8 (8.5~15.9)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>13 (11.3~14.4)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.6 (11~14.1)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.7 (11~14.1)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>246 (190~304)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>237 (177~294)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>104 (100~107)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>104 (101~108)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 (11~21)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 (12~22)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9 (0.7~1.1)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9 (0.7~1.2)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MV during ICU stay</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALINE_FLG</t>
+  </si>
+  <si>
+    <t>DAY_28_FLG</t>
+  </si>
+  <si>
+    <t>0          1</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>100.00     100.00</t>
+  </si>
+  <si>
+    <t>Fisher's exact =</t>
+  </si>
+  <si>
+    <t>344 (43.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>406 (41.3%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>694 (70.5)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>34 (10.1%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>size</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>984 (55.4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discharge from ICU</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
   <si>
     <t>792 (44.6%)</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>NA</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>348 (50%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>51 (35~72)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>56 (40~73)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>53  (35~72)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>54 (38~73)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>aline_flg</t>
-  </si>
-  <si>
-    <t>Odds Ratio</t>
-  </si>
-  <si>
-    <t>Std. Err.</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>P&gt;z</t>
-  </si>
-  <si>
-    <t>[95% Conf.</t>
-  </si>
-  <si>
-    <t>Interval]</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>weight_first</t>
-  </si>
-  <si>
-    <t>sofa_first</t>
-  </si>
-  <si>
-    <t>hour_icu_intime</t>
-  </si>
-  <si>
-    <t>1.chf_flg</t>
-  </si>
-  <si>
-    <t>1.afib_flg</t>
-  </si>
-  <si>
-    <t>1.renal_flg</t>
-  </si>
-  <si>
-    <t>1.liver_flg</t>
-  </si>
-  <si>
-    <t>1.copd_flg</t>
-  </si>
-  <si>
-    <t>1.cad_flg</t>
-  </si>
-  <si>
-    <t>1.stroke_flg</t>
-  </si>
-  <si>
-    <t>1.mal_flg</t>
-  </si>
-  <si>
-    <t>1.resp_flg</t>
-  </si>
-  <si>
-    <t>map_1st</t>
-  </si>
-  <si>
-    <t>hr_1st</t>
-  </si>
-  <si>
-    <t>spo2_1st</t>
-  </si>
-  <si>
-    <t>temp_1st</t>
-  </si>
-  <si>
-    <t>wbc_first</t>
-  </si>
-  <si>
-    <t>hgb_first</t>
-  </si>
-  <si>
-    <t>platelet_first</t>
-  </si>
-  <si>
-    <t>sodium_first</t>
-  </si>
-  <si>
-    <t>potassium_first</t>
-  </si>
-  <si>
-    <t>tco2_first</t>
-  </si>
-  <si>
-    <t>chloride_first</t>
-  </si>
-  <si>
-    <t>bun_first</t>
-  </si>
-  <si>
-    <t>creatinine_first</t>
-  </si>
-  <si>
-    <t>po2_first</t>
-  </si>
-  <si>
-    <t>pco2_first</t>
-  </si>
-  <si>
-    <t>PS model</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>n=1491</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>day_icu_admission</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>MICU (ref) vs CSRU</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mon</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tue</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wed</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thur</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fri</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sat</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUROC: 0.81</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>HL: p=0.4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>12.8 (11.2 ~14.2)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.7 (8~14.8)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.5 (8.4~14.7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>342        351</t>
-  </si>
-  <si>
-    <t>84.44      86.67</t>
-  </si>
-  <si>
-    <t>63         54</t>
-  </si>
-  <si>
-    <t>15.56      13.33</t>
-  </si>
-  <si>
-    <t>405        405</t>
-  </si>
-  <si>
-    <t>140 (138~143)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>140 (137~142)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>238 (184~303)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>238 (186~289)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>24 (22~27)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>24 (21~27)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 (3.6~4.5)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 (3.7~4.4)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>15 (11~22)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switched to DNR and CMO (redo)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>40 (35~46.5)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1075 (361~2385)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1299 (352~2743)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9 (0.5~1.3)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.2 (1.4~3.2)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.75 (0.4~1.3)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.1 (0.6~2.6)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 (1.4~2)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.7 (1.6~5.8)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 (2~7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>7 (5~11)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>3 (2~7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>5 (3~11)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;0.0001</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.8 (1~2.8)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.8 (1.8~4.9)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1 (1.5~5)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.3 (2.3~7.3)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SOFA Score</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHF</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>A-fib</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liver Disease</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Renal Disease</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gender (Female)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>205 (58.9%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>192 (55.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>5 (4~6)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>6 (5~8)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;0.0001</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>5 (4~7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>6 (4~7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Service Unit</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>MICU</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>504 (63.6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>290 (29.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>184 (52.9%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>192 (55.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SICU</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>288 (26.4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>164 (47.1%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>156 (44.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Co-morbidities</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>97 (12.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>116 (11.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>44 (12.6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>36 (10.3%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>82 (10.4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>125 (12.7%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>32 (9.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>28 (3.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>32 (3.3%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>13 (3.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>10 (2.9%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>28 (4.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>61 (6.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>14 (4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>18 (5.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>81 (10.23%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>76 (7.72%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>39 (11.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>51 (6.4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>72 (7.32%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>23 (6.6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>21 (6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>70 (8.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>152 (15.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>33 (9.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>92 (11.6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>164 (16.7%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>51 (14.7%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>278 (35.1%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>287 (29.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>121 (34.7%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>125 (35.9%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.6 (7.8~14.3)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.8 (8.5~15.9)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>13 (11.3~14.4)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>12.6 (11~14.1)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>12.7 (11~14.1)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>246 (190~304)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>237 (177~294)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>104 (100~107)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>104 (101~108)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>15 (11~21)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>16 (12~22)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9 (0.7~1.1)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9 (0.7~1.2)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>MV during ICU stay</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALINE_FLG</t>
-  </si>
-  <si>
-    <t>DAY_28_FLG</t>
-  </si>
-  <si>
-    <t>0          1</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>100.00     100.00</t>
-  </si>
-  <si>
-    <t>Fisher's exact =</t>
-  </si>
-  <si>
-    <t>344 (43.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>406 (41.3%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>694 (70.5)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>34 (10.1%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>size</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>984 (55.4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discharge from ICU</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -955,6 +988,14 @@
   </si>
   <si>
     <t>Age (yr.)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A-fib</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liver Disease</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -962,11 +1003,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8">
@@ -1107,7 +1144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1196,6 +1233,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1555,10 +1595,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:G34"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.42578125" defaultRowHeight="12"/>
@@ -1573,82 +1613,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" customHeight="1">
-      <c r="A1" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>236</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="A1" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="17" customHeight="1" thickBot="1">
-      <c r="A2" s="36"/>
+      <c r="A2" s="37"/>
       <c r="B2" s="12" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" customHeight="1" thickTop="1">
       <c r="A3" s="11" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>1</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D4" s="14">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G4" s="15">
         <v>0.4</v>
@@ -1656,22 +1696,22 @@
     </row>
     <row r="5" spans="1:7" ht="25" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D5" s="15">
         <v>0.36</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G5" s="15">
         <v>0.36</v>
@@ -1679,22 +1719,22 @@
     </row>
     <row r="6" spans="1:7" ht="17" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="G6" s="15">
         <v>0.6</v>
@@ -1702,60 +1742,60 @@
     </row>
     <row r="7" spans="1:7" ht="17" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
-      <c r="D7" s="37" t="s">
-        <v>100</v>
+      <c r="D7" s="38" t="s">
+        <v>106</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="40">
+      <c r="G7" s="41">
         <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="38"/>
+        <v>112</v>
+      </c>
+      <c r="D8" s="39"/>
       <c r="E8" s="15" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="G8" s="41"/>
+        <v>114</v>
+      </c>
+      <c r="G8" s="42"/>
     </row>
     <row r="9" spans="1:7" ht="17" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D9" s="39"/>
+        <v>174</v>
+      </c>
+      <c r="D9" s="40"/>
       <c r="E9" s="15" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="42"/>
+        <v>118</v>
+      </c>
+      <c r="G9" s="43"/>
     </row>
     <row r="10" spans="1:7" ht="24" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -1766,22 +1806,22 @@
     </row>
     <row r="11" spans="1:7" ht="17" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D11" s="15">
         <v>0.7</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="G11" s="15">
         <v>0.4</v>
@@ -1789,22 +1829,22 @@
     </row>
     <row r="12" spans="1:7" ht="17" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>92</v>
+        <v>252</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D12" s="15">
         <v>0.1</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="G12" s="15">
         <v>0.7</v>
@@ -1812,22 +1852,22 @@
     </row>
     <row r="13" spans="1:7" ht="17" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D13" s="15">
         <v>0.8</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G13" s="15">
         <v>0.7</v>
@@ -1835,22 +1875,22 @@
     </row>
     <row r="14" spans="1:7" ht="17" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>93</v>
+        <v>253</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D14" s="15">
         <v>0.2</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="G14" s="15">
         <v>0.6</v>
@@ -1858,22 +1898,22 @@
     </row>
     <row r="15" spans="1:7" ht="17" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D15" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G15" s="15">
         <v>0.5</v>
@@ -1881,22 +1921,22 @@
     </row>
     <row r="16" spans="1:7" ht="17" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D16" s="15">
         <v>0.5</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="G16" s="15">
         <v>0.8</v>
@@ -1904,22 +1944,22 @@
     </row>
     <row r="17" spans="1:7" ht="17" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D17" s="14">
         <v>1E-4</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="G17" s="15">
         <v>1</v>
@@ -1927,22 +1967,22 @@
     </row>
     <row r="18" spans="1:7" ht="17" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D18" s="14">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G18" s="15">
         <v>0.6</v>
@@ -1950,171 +1990,171 @@
     </row>
     <row r="19" spans="1:7" ht="26" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D19" s="14">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G19" s="15">
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17" customHeight="1">
-      <c r="A20" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="1:7" ht="17" customHeight="1">
+    <row r="20" spans="1:7" ht="26" customHeight="1">
+      <c r="A20" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="34">
+        <v>0.01</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="26" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>215</v>
+        <v>0</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>146</v>
+        <v>7</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c r="D21" s="34">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="G21" s="15">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17" customHeight="1">
-      <c r="A22" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D22" s="14">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="G22" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="A22" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" ht="17" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="D23" s="15">
-        <v>0.01</v>
+        <v>153</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G23" s="15">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>62</v>
+        <v>154</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="15">
-        <v>7.0000000000000001E-3</v>
+        <v>155</v>
+      </c>
+      <c r="D24" s="14">
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>63</v>
+        <v>156</v>
       </c>
       <c r="G24" s="15">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="D25" s="15">
-        <v>0.77</v>
+        <v>0.01</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G25" s="15">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D26" s="15">
-        <v>0.05</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G26" s="15">
         <v>0.6</v>
@@ -2122,175 +2162,222 @@
     </row>
     <row r="27" spans="1:7" ht="17" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>194</v>
+        <v>227</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>153</v>
+        <v>75</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D27" s="14">
-        <v>2.9999999999999997E-4</v>
+        <v>76</v>
+      </c>
+      <c r="D27" s="15">
+        <v>0.77</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>153</v>
+        <v>75</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
       <c r="G27" s="15">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>195</v>
+        <v>228</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>155</v>
+        <v>73</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D28" s="14">
-        <v>0.02</v>
+        <v>74</v>
+      </c>
+      <c r="D28" s="15">
+        <v>0.05</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>156</v>
+        <v>74</v>
       </c>
       <c r="G28" s="15">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="D29" s="15">
-        <v>0.6</v>
+        <v>160</v>
+      </c>
+      <c r="D29" s="14">
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G29" s="15">
-        <v>7.0000000000000007E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" customHeight="1">
       <c r="A30" s="10" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>221</v>
+        <v>161</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="D30" s="15">
-        <v>0.5</v>
+        <v>162</v>
+      </c>
+      <c r="D30" s="14">
+        <v>0.02</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>223</v>
+        <v>77</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>224</v>
+        <v>162</v>
       </c>
       <c r="G30" s="15">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>225</v>
+        <v>163</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D31" s="14">
+        <v>163</v>
+      </c>
+      <c r="D31" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" customHeight="1">
+      <c r="A32" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D32" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="G32" s="15">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" customHeight="1">
+      <c r="A33" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D33" s="14">
         <v>0.02</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G31" s="15">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="17" customHeight="1">
-      <c r="A32" s="10"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-    </row>
-    <row r="33" spans="1:7" ht="27" customHeight="1">
-      <c r="A33" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>100</v>
-      </c>
       <c r="E33" s="15" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>232</v>
+        <v>79</v>
       </c>
       <c r="G33" s="15">
         <v>0.2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="38" customHeight="1">
-      <c r="A34" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="G34" s="15">
+    <row r="34" spans="1:7" ht="17" customHeight="1">
+      <c r="A34" s="10"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+    </row>
+    <row r="35" spans="1:7" ht="27" customHeight="1">
+      <c r="A35" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="G35" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="38" customHeight="1">
+      <c r="A36" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G36" s="15">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="5">
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="B1:D1"/>
@@ -2314,7 +2401,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
@@ -2328,24 +2415,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="22" customHeight="1" thickBot="1">
       <c r="A1" s="23" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" thickTop="1">
       <c r="A2" s="21" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B2" s="25">
         <v>0.152</v>
@@ -2354,7 +2441,7 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E2" s="22">
         <v>0.9</v>
@@ -2362,7 +2449,7 @@
     </row>
     <row r="3" spans="1:5" ht="29" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -2371,33 +2458,33 @@
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="E5" s="20">
         <v>6.0000000000000001E-3</v>
@@ -2405,33 +2492,33 @@
     </row>
     <row r="6" spans="1:5" ht="29" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="E7" s="20">
         <v>3.0000000000000001E-3</v>
@@ -2439,33 +2526,33 @@
     </row>
     <row r="8" spans="1:5" ht="29" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E9" s="20">
         <v>2.9999999999999997E-4</v>
@@ -2473,39 +2560,40 @@
     </row>
     <row r="10" spans="1:5" ht="29" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="E11" s="20">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2533,23 +2621,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2557,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>693</v>
@@ -2565,7 +2653,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>85.56</v>
@@ -2579,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C10">
         <v>117</v>
@@ -2587,7 +2675,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C11">
         <v>14.44</v>
@@ -2595,10 +2683,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C13">
         <v>810</v>
@@ -2606,7 +2694,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C14">
         <v>100</v>
@@ -2617,13 +2705,14 @@
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C16" s="5">
         <v>0.42399999999999999</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2652,38 +2741,38 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3">
         <v>0.99664870000000005</v>
@@ -2706,7 +2795,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>1.000894</v>
@@ -2729,7 +2818,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3">
         <v>1.59127</v>
@@ -2752,7 +2841,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3">
         <v>7.2156000000000002</v>
@@ -2781,7 +2870,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2790,7 +2879,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3">
         <v>1.5041310000000001</v>
@@ -2813,7 +2902,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3">
         <v>1.183298</v>
@@ -2836,7 +2925,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B13" s="3">
         <v>1.5754729999999999</v>
@@ -2859,7 +2948,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B14" s="3">
         <v>1.4919450000000001</v>
@@ -2882,7 +2971,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B15" s="3">
         <v>1.9040029999999999</v>
@@ -2905,7 +2994,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B16" s="3">
         <v>1.127912</v>
@@ -2934,7 +3023,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B18" s="3">
         <v>1.0259119999999999</v>
@@ -2957,7 +3046,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3">
         <v>1.7799700000000001</v>
@@ -2980,7 +3069,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B20" s="3">
         <v>0.97763770000000005</v>
@@ -3003,7 +3092,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3">
         <v>1.537355</v>
@@ -3026,7 +3115,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B22" s="3">
         <v>0.36014439999999998</v>
@@ -3049,7 +3138,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B23" s="3">
         <v>0.78372209999999998</v>
@@ -3072,7 +3161,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3">
         <v>0.95840420000000004</v>
@@ -3095,7 +3184,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B25" s="3">
         <v>1.382242</v>
@@ -3118,7 +3207,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B26" s="3">
         <v>1.1597500000000001</v>
@@ -3141,7 +3230,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B27" s="3">
         <v>1.016337</v>
@@ -3164,7 +3253,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B28" s="3">
         <v>1.007226</v>
@@ -3187,7 +3276,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B29" s="3">
         <v>1.0063120000000001</v>
@@ -3210,7 +3299,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3">
         <v>0.97394990000000004</v>
@@ -3233,7 +3322,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B31" s="3">
         <v>1.0002230000000001</v>
@@ -3256,7 +3345,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B32" s="3">
         <v>1.032224</v>
@@ -3279,7 +3368,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3">
         <v>0.95359110000000002</v>
@@ -3302,7 +3391,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B34" s="3">
         <v>0.99973749999999995</v>
@@ -3325,7 +3414,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B35" s="4">
         <v>0.92980370000000001</v>
@@ -3348,7 +3437,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B36" s="4">
         <v>1.0222789999999999</v>
@@ -3371,7 +3460,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B37" s="4">
         <v>1.023301</v>
@@ -3394,7 +3483,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B38" s="4">
         <v>1.055034</v>
@@ -3417,7 +3506,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B39" s="4">
         <v>1.005822</v>
@@ -3440,7 +3529,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B40" s="4">
         <v>0.76309660000000001</v>
@@ -3463,7 +3552,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B41" s="4">
         <v>1.0007079999999999</v>
@@ -3486,7 +3575,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B42" s="4">
         <v>0.99573080000000003</v>
@@ -3509,15 +3598,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3533,7 +3623,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3544,36 +3634,36 @@
   <sheetData>
     <row r="1" spans="1:9" ht="27" thickBot="1">
       <c r="A1" s="23" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="27" thickTop="1">
       <c r="A2" s="21" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B2" s="25">
         <v>0.152</v>
@@ -3582,86 +3672,86 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E2" s="22">
         <v>0.9</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="G2" s="30">
         <v>0.72</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="39">
       <c r="A3" s="17" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="20"/>
       <c r="E3" s="19"/>
       <c r="F3" s="16" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="G3" s="32">
         <v>0.71</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39">
       <c r="A4" s="18" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="G4" s="32">
         <v>0.74</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="39">
       <c r="A5" s="18" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="E5" s="20">
         <v>0.3</v>
@@ -3672,6 +3762,30 @@
       <c r="I5" s="20"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Jan 18th 2015 updates
</commit_message>
<xml_diff>
--- a/Figures_Tables/result_tables/tables.xlsx
+++ b/Figures_Tables/result_tables/tables.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="13860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 2_old" sheetId="2" r:id="rId2"/>
+    <sheet name="Table 2" sheetId="2" r:id="rId2"/>
     <sheet name="Sensitivity study" sheetId="3" r:id="rId3"/>
     <sheet name="Ps model" sheetId="4" r:id="rId4"/>
-    <sheet name="Table2_New" sheetId="5" r:id="rId5"/>
+    <sheet name="Competing risk" sheetId="5" r:id="rId5"/>
     <sheet name="MV_indication_comparison" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="130000" concurrentCalc="0"/>
@@ -24,651 +24,101 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="254">
-  <si>
-    <t>Pneumonia</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>16 (4.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>18 (5.4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>67 (20%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>68 (20.3%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>33 (4.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>70 (7.1%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>147 (18.6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>152 (15.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>348 (50%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>51 (35~72)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>56 (40~73)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>53  (35~72)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>54 (38~73)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>aline_flg</t>
-  </si>
-  <si>
-    <t>Odds Ratio</t>
-  </si>
-  <si>
-    <t>Std. Err.</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>P&gt;z</t>
-  </si>
-  <si>
-    <t>[95% Conf.</t>
-  </si>
-  <si>
-    <t>Interval]</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>weight_first</t>
-  </si>
-  <si>
-    <t>sofa_first</t>
-  </si>
-  <si>
-    <t>hour_icu_intime</t>
-  </si>
-  <si>
-    <t>1.chf_flg</t>
-  </si>
-  <si>
-    <t>1.afib_flg</t>
-  </si>
-  <si>
-    <t>1.renal_flg</t>
-  </si>
-  <si>
-    <t>1.liver_flg</t>
-  </si>
-  <si>
-    <t>1.copd_flg</t>
-  </si>
-  <si>
-    <t>1.cad_flg</t>
-  </si>
-  <si>
-    <t>1.stroke_flg</t>
-  </si>
-  <si>
-    <t>1.mal_flg</t>
-  </si>
-  <si>
-    <t>1.resp_flg</t>
-  </si>
-  <si>
-    <t>map_1st</t>
-  </si>
-  <si>
-    <t>hr_1st</t>
-  </si>
-  <si>
-    <t>spo2_1st</t>
-  </si>
-  <si>
-    <t>temp_1st</t>
-  </si>
-  <si>
-    <t>wbc_first</t>
-  </si>
-  <si>
-    <t>hgb_first</t>
-  </si>
-  <si>
-    <t>platelet_first</t>
-  </si>
-  <si>
-    <t>sodium_first</t>
-  </si>
-  <si>
-    <t>potassium_first</t>
-  </si>
-  <si>
-    <t>tco2_first</t>
-  </si>
-  <si>
-    <t>chloride_first</t>
-  </si>
-  <si>
-    <t>bun_first</t>
-  </si>
-  <si>
-    <t>creatinine_first</t>
-  </si>
-  <si>
-    <t>po2_first</t>
-  </si>
-  <si>
-    <t>pco2_first</t>
-  </si>
-  <si>
-    <t>PS model</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>n=1491</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>day_icu_admission</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>MICU (ref) vs CSRU</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mon</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tue</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wed</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thur</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fri</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sat</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUROC: 0.81</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>HL: p=0.4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>12.8 (11.2 ~14.2)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.7 (8~14.8)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.5 (8.4~14.7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>342        351</t>
-  </si>
-  <si>
-    <t>84.44      86.67</t>
-  </si>
-  <si>
-    <t>63         54</t>
-  </si>
-  <si>
-    <t>15.56      13.33</t>
-  </si>
-  <si>
-    <t>405        405</t>
-  </si>
-  <si>
-    <t>140 (138~143)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>140 (137~142)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>238 (184~303)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>238 (186~289)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>24 (22~27)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>24 (21~27)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 (3.6~4.5)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 (3.7~4.4)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>15 (11~22)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switched to DNR and CMO (redo)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>40 (35~46.5)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1075 (361~2385)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1299 (352~2743)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9 (0.5~1.3)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.2 (1.4~3.2)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.75 (0.4~1.3)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.1 (0.6~2.6)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 (1.4~2)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.7 (1.6~5.8)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 (2~7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>7 (5~11)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>3 (2~7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>5 (3~11)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;0.0001</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.8 (1~2.8)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.8 (1.8~4.9)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1 (1.5~5)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.3 (2.3~7.3)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SOFA Score</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHF</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ARDS</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Renal Disease</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gender (Female)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>205 (58.9%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>192 (55.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>5 (4~6)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>6 (5~8)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;0.0001</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>5 (4~7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>6 (4~7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Service Unit</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>MICU</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>504 (63.6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>290 (29.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>184 (52.9%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>192 (55.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SICU</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>288 (26.4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>164 (47.1%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>156 (44.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Co-morbidities</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>97 (12.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>116 (11.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>44 (12.6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>36 (10.3%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>82 (10.4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>125 (12.7%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>32 (9.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>28 (3.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>32 (3.3%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>13 (3.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>10 (2.9%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>28 (4.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>61 (6.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>14 (4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>18 (5.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>81 (10.23%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>76 (7.72%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>39 (11.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>51 (6.4%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>72 (7.32%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>23 (6.6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>21 (6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>70 (8.8%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>152 (15.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>33 (9.5%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>92 (11.6%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>164 (16.7%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>51 (14.7%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>278 (35.1%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>287 (29.2%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>121 (34.7%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>125 (35.9%)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.6 (7.8~14.3)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.8 (8.5~15.9)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>13 (11.3~14.4)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>12.6 (11~14.1)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>12.7 (11~14.1)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>246 (190~304)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>237 (177~294)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>104 (100~107)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>104 (101~108)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>15 (11~21)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>16 (12~22)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9 (0.7~1.1)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9 (0.7~1.2)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>MV during ICU stay</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALINE_FLG</t>
-  </si>
-  <si>
-    <t>DAY_28_FLG</t>
-  </si>
-  <si>
-    <t>0          1</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>100.00     100.00</t>
-  </si>
-  <si>
-    <t>Fisher's exact =</t>
-  </si>
-  <si>
-    <t>344 (43.5%)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="254">
+  <si>
+    <t>Matched Cohort (696)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-IAC</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IAC</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>p-value</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>lab tests</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age (yr.)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A-fib</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liver Disease</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2 (+/-1.4)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.7 (+/-3.1)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.6 (+/-2.2)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.2 (+/-5.3)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.7 (+/-4.8)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.4 (+/-7.5)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4 (+/-4.5)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.6 (+/-7)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 (+/-1)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1 (+/-2.6)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 (+/-1.6)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.3 (+/-5.3)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 (+/-0.8)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.4 (+/-1.4)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1564 (+/-1459)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1758 (+/-1852)</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -967,35 +417,585 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Matched Cohort (696)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Non-IAC</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IAC</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>p-value</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>lab tests</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Age (yr.)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>A-fib</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liver Disease</t>
+    <t>&lt;0.0001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOFA Score</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHF</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARDS</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Renal Disease</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gender (Female)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>205 (58.9%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>192 (55.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 (4~6)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 (5~8)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;0.0001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 (4~7)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 (4~7)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Service Unit</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MICU</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>504 (63.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>290 (29.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>184 (52.9%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>192 (55.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SICU</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>288 (26.4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>164 (47.1%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>156 (44.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Co-morbidities</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>97 (12.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>116 (11.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>44 (12.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>36 (10.3%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>82 (10.4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>125 (12.7%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>32 (9.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>28 (3.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>32 (3.3%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>13 (3.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 (2.9%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>28 (4.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>61 (6.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>14 (4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 (5.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>81 (10.23%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>76 (7.72%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>39 (11.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>51 (6.4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>72 (7.32%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>23 (6.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>21 (6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>70 (8.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>152 (15.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>33 (9.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>92 (11.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>164 (16.7%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>51 (14.7%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>278 (35.1%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>287 (29.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>121 (34.7%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>125 (35.9%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.6 (7.8~14.3)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.8 (8.5~15.9)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>13 (11.3~14.4)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.6 (11~14.1)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.7 (11~14.1)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>246 (190~304)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>237 (177~294)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>104 (100~107)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>104 (101~108)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 (11~21)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 (12~22)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9 (0.7~1.1)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9 (0.7~1.2)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MV during ICU stay</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALINE_FLG</t>
+  </si>
+  <si>
+    <t>DAY_28_FLG</t>
+  </si>
+  <si>
+    <t>0          1</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>100.00     100.00</t>
+  </si>
+  <si>
+    <t>Fisher's exact =</t>
+  </si>
+  <si>
+    <t>344 (43.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pneumonia</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 (4.8%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 (5.4%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>67 (20%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>68 (20.3%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>33 (4.2%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>70 (7.1%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>147 (18.6%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>152 (15.5%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>348 (50%)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>51 (35~72)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>56 (40~73)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>53  (35~72)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>54 (38~73)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>aline_flg</t>
+  </si>
+  <si>
+    <t>Odds Ratio</t>
+  </si>
+  <si>
+    <t>Std. Err.</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>P&gt;z</t>
+  </si>
+  <si>
+    <t>[95% Conf.</t>
+  </si>
+  <si>
+    <t>Interval]</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>weight_first</t>
+  </si>
+  <si>
+    <t>sofa_first</t>
+  </si>
+  <si>
+    <t>hour_icu_intime</t>
+  </si>
+  <si>
+    <t>1.chf_flg</t>
+  </si>
+  <si>
+    <t>1.afib_flg</t>
+  </si>
+  <si>
+    <t>1.renal_flg</t>
+  </si>
+  <si>
+    <t>1.liver_flg</t>
+  </si>
+  <si>
+    <t>1.copd_flg</t>
+  </si>
+  <si>
+    <t>1.cad_flg</t>
+  </si>
+  <si>
+    <t>1.stroke_flg</t>
+  </si>
+  <si>
+    <t>1.mal_flg</t>
+  </si>
+  <si>
+    <t>1.resp_flg</t>
+  </si>
+  <si>
+    <t>map_1st</t>
+  </si>
+  <si>
+    <t>hr_1st</t>
+  </si>
+  <si>
+    <t>spo2_1st</t>
+  </si>
+  <si>
+    <t>temp_1st</t>
+  </si>
+  <si>
+    <t>wbc_first</t>
+  </si>
+  <si>
+    <t>hgb_first</t>
+  </si>
+  <si>
+    <t>platelet_first</t>
+  </si>
+  <si>
+    <t>sodium_first</t>
+  </si>
+  <si>
+    <t>potassium_first</t>
+  </si>
+  <si>
+    <t>tco2_first</t>
+  </si>
+  <si>
+    <t>chloride_first</t>
+  </si>
+  <si>
+    <t>bun_first</t>
+  </si>
+  <si>
+    <t>creatinine_first</t>
+  </si>
+  <si>
+    <t>po2_first</t>
+  </si>
+  <si>
+    <t>pco2_first</t>
+  </si>
+  <si>
+    <t>PS model</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>n=1491</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>day_icu_admission</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MICU (ref) vs CSRU</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mon</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tue</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wed</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thur</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fri</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sat</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUROC: 0.81</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HL: p=0.4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.8 (11.2 ~14.2)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.7 (8~14.8)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.5 (8.4~14.7)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>342        351</t>
+  </si>
+  <si>
+    <t>84.44      86.67</t>
+  </si>
+  <si>
+    <t>63         54</t>
+  </si>
+  <si>
+    <t>15.56      13.33</t>
+  </si>
+  <si>
+    <t>405        405</t>
+  </si>
+  <si>
+    <t>140 (138~143)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>140 (137~142)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>238 (184~303)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>238 (186~289)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>24 (22~27)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>24 (21~27)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 (3.6~4.5)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 (3.7~4.4)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 (11~22)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switched to DNR and CMO (redo)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>40 (35~46.5)</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1003,7 +1003,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8">
@@ -1597,7 +1601,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="H21" sqref="H21:J34"/>
     </sheetView>
   </sheetViews>
@@ -1614,15 +1618,15 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" customHeight="1">
       <c r="A1" s="36" t="s">
-        <v>245</v>
+        <v>96</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>244</v>
+        <v>95</v>
       </c>
       <c r="C1" s="35"/>
       <c r="D1" s="35"/>
       <c r="E1" s="35" t="s">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="F1" s="35"/>
       <c r="G1" s="35"/>
@@ -1630,65 +1634,65 @@
     <row r="2" spans="1:7" ht="17" customHeight="1" thickBot="1">
       <c r="A2" s="37"/>
       <c r="B2" s="12" t="s">
-        <v>247</v>
+        <v>1</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>248</v>
+        <v>2</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>249</v>
+        <v>3</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>247</v>
+        <v>1</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>248</v>
+        <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>249</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" customHeight="1" thickTop="1">
       <c r="A3" s="11" t="s">
-        <v>176</v>
+        <v>27</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>179</v>
+        <v>30</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>180</v>
+        <v>31</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>9</v>
+        <v>183</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>9</v>
+        <v>183</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>180</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>251</v>
+        <v>5</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>10</v>
+        <v>184</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="D4" s="14">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>12</v>
+        <v>186</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>13</v>
+        <v>187</v>
       </c>
       <c r="G4" s="15">
         <v>0.4</v>
@@ -1696,22 +1700,22 @@
     </row>
     <row r="5" spans="1:7" ht="25" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>173</v>
+        <v>24</v>
       </c>
       <c r="D5" s="15">
         <v>0.36</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G5" s="15">
         <v>0.36</v>
@@ -1719,22 +1723,22 @@
     </row>
     <row r="6" spans="1:7" ht="17" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G6" s="15">
         <v>0.6</v>
@@ -1742,12 +1746,12 @@
     </row>
     <row r="7" spans="1:7" ht="17" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="38" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -1757,45 +1761,45 @@
     </row>
     <row r="8" spans="1:7" ht="17" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D8" s="39"/>
       <c r="E8" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G8" s="42"/>
     </row>
     <row r="9" spans="1:7" ht="17" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>174</v>
+        <v>25</v>
       </c>
       <c r="D9" s="40"/>
       <c r="E9" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G9" s="43"/>
     </row>
     <row r="10" spans="1:7" ht="24" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -1806,22 +1810,22 @@
     </row>
     <row r="11" spans="1:7" ht="17" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D11" s="15">
         <v>0.7</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G11" s="15">
         <v>0.4</v>
@@ -1829,22 +1833,22 @@
     </row>
     <row r="12" spans="1:7" ht="17" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>252</v>
+        <v>6</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D12" s="15">
         <v>0.1</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G12" s="15">
         <v>0.7</v>
@@ -1852,22 +1856,22 @@
     </row>
     <row r="13" spans="1:7" ht="17" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D13" s="15">
         <v>0.8</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G13" s="15">
         <v>0.7</v>
@@ -1875,22 +1879,22 @@
     </row>
     <row r="14" spans="1:7" ht="17" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>253</v>
+        <v>7</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D14" s="15">
         <v>0.2</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G14" s="15">
         <v>0.6</v>
@@ -1898,22 +1902,22 @@
     </row>
     <row r="15" spans="1:7" ht="17" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>218</v>
+        <v>69</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D15" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G15" s="15">
         <v>0.5</v>
@@ -1921,22 +1925,22 @@
     </row>
     <row r="16" spans="1:7" ht="17" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>219</v>
+        <v>70</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D16" s="15">
         <v>0.5</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G16" s="15">
         <v>0.8</v>
@@ -1944,22 +1948,22 @@
     </row>
     <row r="17" spans="1:7" ht="17" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>220</v>
+        <v>71</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D17" s="14">
         <v>1E-4</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G17" s="15">
         <v>1</v>
@@ -1967,22 +1971,22 @@
     </row>
     <row r="18" spans="1:7" ht="17" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>221</v>
+        <v>72</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D18" s="14">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G18" s="15">
         <v>0.6</v>
@@ -1990,22 +1994,22 @@
     </row>
     <row r="19" spans="1:7" ht="26" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>222</v>
+        <v>73</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D19" s="14">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G19" s="15">
         <v>0.8</v>
@@ -2013,22 +2017,22 @@
     </row>
     <row r="20" spans="1:7" ht="26" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>6</v>
+        <v>180</v>
       </c>
       <c r="D20" s="34">
         <v>0.01</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="G20" s="15">
         <v>0.8</v>
@@ -2036,22 +2040,22 @@
     </row>
     <row r="21" spans="1:7" ht="26" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>8</v>
+        <v>182</v>
       </c>
       <c r="D21" s="34">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>3</v>
+        <v>177</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>4</v>
+        <v>178</v>
       </c>
       <c r="G21" s="15">
         <v>1</v>
@@ -2059,7 +2063,7 @@
     </row>
     <row r="22" spans="1:7" ht="17" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>250</v>
+        <v>4</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -2070,22 +2074,22 @@
     </row>
     <row r="23" spans="1:7" ht="17" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>223</v>
+        <v>74</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>62</v>
+        <v>236</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>63</v>
+        <v>237</v>
       </c>
       <c r="G23" s="15">
         <v>0.3</v>
@@ -2093,22 +2097,22 @@
     </row>
     <row r="24" spans="1:7" ht="17" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>224</v>
+        <v>75</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D24" s="14">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>61</v>
+        <v>235</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G24" s="15">
         <v>0.5</v>
@@ -2116,22 +2120,22 @@
     </row>
     <row r="25" spans="1:7" ht="17" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>225</v>
+        <v>76</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D25" s="15">
         <v>0.01</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>71</v>
+        <v>245</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>72</v>
+        <v>246</v>
       </c>
       <c r="G25" s="15">
         <v>0.7</v>
@@ -2139,22 +2143,22 @@
     </row>
     <row r="26" spans="1:7" ht="17" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>226</v>
+        <v>77</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>69</v>
+        <v>243</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
       <c r="D26" s="15">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>69</v>
+        <v>243</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
       <c r="G26" s="15">
         <v>0.6</v>
@@ -2162,22 +2166,22 @@
     </row>
     <row r="27" spans="1:7" ht="17" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>227</v>
+        <v>78</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>75</v>
+        <v>249</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>76</v>
+        <v>250</v>
       </c>
       <c r="D27" s="15">
         <v>0.77</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>75</v>
+        <v>249</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>76</v>
+        <v>250</v>
       </c>
       <c r="G27" s="15">
         <v>0.8</v>
@@ -2185,22 +2189,22 @@
     </row>
     <row r="28" spans="1:7" ht="17" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>228</v>
+        <v>79</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>73</v>
+        <v>247</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>74</v>
+        <v>248</v>
       </c>
       <c r="D28" s="15">
         <v>0.05</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>73</v>
+        <v>247</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>74</v>
+        <v>248</v>
       </c>
       <c r="G28" s="15">
         <v>0.6</v>
@@ -2208,22 +2212,22 @@
     </row>
     <row r="29" spans="1:7" ht="17" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>202</v>
+        <v>53</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D29" s="14">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G29" s="15">
         <v>1</v>
@@ -2231,22 +2235,22 @@
     </row>
     <row r="30" spans="1:7" ht="17" customHeight="1">
       <c r="A30" s="10" t="s">
-        <v>203</v>
+        <v>54</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D30" s="14">
         <v>0.02</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>77</v>
+        <v>251</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G30" s="15">
         <v>0.3</v>
@@ -2254,22 +2258,22 @@
     </row>
     <row r="31" spans="1:7" ht="17" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>204</v>
+        <v>55</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D31" s="15">
         <v>0.6</v>
       </c>
       <c r="E31" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F31" s="15" t="s">
         <v>164</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="G31" s="15">
         <v>7.0000000000000007E-2</v>
@@ -2277,22 +2281,22 @@
     </row>
     <row r="32" spans="1:7" ht="17" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>205</v>
+        <v>56</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>229</v>
+        <v>80</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>230</v>
+        <v>81</v>
       </c>
       <c r="D32" s="15">
         <v>0.5</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>231</v>
+        <v>82</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>232</v>
+        <v>83</v>
       </c>
       <c r="G32" s="15">
         <v>0.7</v>
@@ -2300,22 +2304,22 @@
     </row>
     <row r="33" spans="1:7" ht="17" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>206</v>
+        <v>57</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>233</v>
+        <v>84</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>234</v>
+        <v>85</v>
       </c>
       <c r="D33" s="14">
         <v>0.02</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>235</v>
+        <v>86</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>79</v>
+        <v>253</v>
       </c>
       <c r="G33" s="15">
         <v>0.2</v>
@@ -2332,22 +2336,22 @@
     </row>
     <row r="35" spans="1:7" ht="27" customHeight="1">
       <c r="A35" s="10" t="s">
-        <v>236</v>
+        <v>87</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>237</v>
+        <v>88</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>238</v>
+        <v>89</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>239</v>
+        <v>90</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>240</v>
+        <v>91</v>
       </c>
       <c r="G35" s="15">
         <v>0.2</v>
@@ -2355,29 +2359,28 @@
     </row>
     <row r="36" spans="1:7" ht="38" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>78</v>
+        <v>252</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>241</v>
+        <v>92</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>242</v>
+        <v>93</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>243</v>
+        <v>94</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>175</v>
+        <v>26</v>
       </c>
       <c r="G36" s="15">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="5">
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="B1:D1"/>
@@ -2401,8 +2404,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:E11"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2415,24 +2418,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="22" customHeight="1" thickBot="1">
       <c r="A1" s="23" t="s">
-        <v>195</v>
+        <v>46</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>191</v>
+        <v>42</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>192</v>
+        <v>43</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>193</v>
+        <v>44</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" thickTop="1">
       <c r="A2" s="21" t="s">
-        <v>189</v>
+        <v>40</v>
       </c>
       <c r="B2" s="25">
         <v>0.152</v>
@@ -2441,7 +2444,7 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="E2" s="22">
         <v>0.9</v>
@@ -2449,7 +2452,7 @@
     </row>
     <row r="3" spans="1:5" ht="29" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -2458,33 +2461,33 @@
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>214</v>
+        <v>65</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>207</v>
+        <v>58</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>196</v>
+        <v>47</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="E5" s="20">
         <v>6.0000000000000001E-3</v>
@@ -2492,33 +2495,33 @@
     </row>
     <row r="6" spans="1:5" ht="29" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>215</v>
+        <v>66</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>209</v>
+        <v>60</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>210</v>
+        <v>61</v>
       </c>
       <c r="E7" s="20">
         <v>3.0000000000000001E-3</v>
@@ -2526,33 +2529,33 @@
     </row>
     <row r="8" spans="1:5" ht="29" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>211</v>
+        <v>62</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>84</v>
+        <v>16</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>216</v>
+        <v>67</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>198</v>
+        <v>49</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>217</v>
+        <v>68</v>
       </c>
       <c r="E9" s="20">
         <v>2.9999999999999997E-4</v>
@@ -2560,40 +2563,39 @@
     </row>
     <row r="10" spans="1:5" ht="29" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>212</v>
+        <v>63</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>186</v>
+        <v>37</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>213</v>
+        <v>64</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>187</v>
+        <v>38</v>
       </c>
       <c r="E11" s="20">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2621,23 +2623,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2645,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>238</v>
       </c>
       <c r="C7">
         <v>693</v>
@@ -2653,7 +2655,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>65</v>
+        <v>239</v>
       </c>
       <c r="C8">
         <v>85.56</v>
@@ -2667,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>240</v>
       </c>
       <c r="C10">
         <v>117</v>
@@ -2675,7 +2677,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="5" t="s">
-        <v>67</v>
+        <v>241</v>
       </c>
       <c r="C11">
         <v>14.44</v>
@@ -2683,10 +2685,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>242</v>
       </c>
       <c r="C13">
         <v>810</v>
@@ -2694,7 +2696,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C14">
         <v>100</v>
@@ -2705,14 +2707,13 @@
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C16" s="5">
         <v>0.42399999999999999</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2741,38 +2742,38 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>223</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>192</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>193</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>195</v>
       </c>
       <c r="B5" s="3">
         <v>0.99664870000000005</v>
@@ -2795,7 +2796,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>196</v>
       </c>
       <c r="B6" s="3">
         <v>1.000894</v>
@@ -2818,7 +2819,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>197</v>
       </c>
       <c r="B7" s="3">
         <v>1.59127</v>
@@ -2841,7 +2842,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="B8" s="3">
         <v>7.2156000000000002</v>
@@ -2870,7 +2871,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>225</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2879,7 +2880,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>227</v>
       </c>
       <c r="B11" s="3">
         <v>1.5041310000000001</v>
@@ -2902,7 +2903,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>228</v>
       </c>
       <c r="B12" s="3">
         <v>1.183298</v>
@@ -2925,7 +2926,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>229</v>
       </c>
       <c r="B13" s="3">
         <v>1.5754729999999999</v>
@@ -2948,7 +2949,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>230</v>
       </c>
       <c r="B14" s="3">
         <v>1.4919450000000001</v>
@@ -2971,7 +2972,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>231</v>
       </c>
       <c r="B15" s="3">
         <v>1.9040029999999999</v>
@@ -2994,7 +2995,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>232</v>
       </c>
       <c r="B16" s="3">
         <v>1.127912</v>
@@ -3023,7 +3024,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>198</v>
       </c>
       <c r="B18" s="3">
         <v>1.0259119999999999</v>
@@ -3046,7 +3047,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>199</v>
       </c>
       <c r="B19" s="3">
         <v>1.7799700000000001</v>
@@ -3069,7 +3070,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>200</v>
       </c>
       <c r="B20" s="3">
         <v>0.97763770000000005</v>
@@ -3092,7 +3093,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>201</v>
       </c>
       <c r="B21" s="3">
         <v>1.537355</v>
@@ -3115,7 +3116,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
       <c r="B22" s="3">
         <v>0.36014439999999998</v>
@@ -3138,7 +3139,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="B23" s="3">
         <v>0.78372209999999998</v>
@@ -3161,7 +3162,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>204</v>
       </c>
       <c r="B24" s="3">
         <v>0.95840420000000004</v>
@@ -3184,7 +3185,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>205</v>
       </c>
       <c r="B25" s="3">
         <v>1.382242</v>
@@ -3207,7 +3208,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>206</v>
       </c>
       <c r="B26" s="3">
         <v>1.1597500000000001</v>
@@ -3230,7 +3231,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>207</v>
       </c>
       <c r="B27" s="3">
         <v>1.016337</v>
@@ -3253,7 +3254,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="B28" s="3">
         <v>1.007226</v>
@@ -3276,7 +3277,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>209</v>
       </c>
       <c r="B29" s="3">
         <v>1.0063120000000001</v>
@@ -3299,7 +3300,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>210</v>
       </c>
       <c r="B30" s="3">
         <v>0.97394990000000004</v>
@@ -3322,7 +3323,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>211</v>
       </c>
       <c r="B31" s="3">
         <v>1.0002230000000001</v>
@@ -3345,7 +3346,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>212</v>
       </c>
       <c r="B32" s="3">
         <v>1.032224</v>
@@ -3368,7 +3369,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>213</v>
       </c>
       <c r="B33" s="3">
         <v>0.95359110000000002</v>
@@ -3391,7 +3392,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>214</v>
       </c>
       <c r="B34" s="3">
         <v>0.99973749999999995</v>
@@ -3414,7 +3415,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>215</v>
       </c>
       <c r="B35" s="4">
         <v>0.92980370000000001</v>
@@ -3437,7 +3438,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>216</v>
       </c>
       <c r="B36" s="4">
         <v>1.0222789999999999</v>
@@ -3460,7 +3461,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>217</v>
       </c>
       <c r="B37" s="4">
         <v>1.023301</v>
@@ -3483,7 +3484,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>218</v>
       </c>
       <c r="B38" s="4">
         <v>1.055034</v>
@@ -3506,7 +3507,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>219</v>
       </c>
       <c r="B39" s="4">
         <v>1.005822</v>
@@ -3529,7 +3530,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>220</v>
       </c>
       <c r="B40" s="4">
         <v>0.76309660000000001</v>
@@ -3552,7 +3553,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>221</v>
       </c>
       <c r="B41" s="4">
         <v>1.0007079999999999</v>
@@ -3575,7 +3576,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>222</v>
       </c>
       <c r="B42" s="4">
         <v>0.99573080000000003</v>
@@ -3598,16 +3599,15 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3621,10 +3621,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A3:D12"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3632,137 +3632,72 @@
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" thickBot="1">
-      <c r="A1" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="27" thickTop="1">
-      <c r="A2" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="25">
-        <v>0.152</v>
-      </c>
-      <c r="C2" s="25">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="E2" s="22">
-        <v>0.9</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="G2" s="30">
+    <row r="3" spans="1:4" ht="27" thickBot="1">
+      <c r="A3" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27" thickTop="1">
+      <c r="A4" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="30">
         <v>0.72</v>
       </c>
-      <c r="H2" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="39">
-      <c r="A3" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="G3" s="32">
+      <c r="C4" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="39">
+      <c r="A5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="32">
         <v>0.71</v>
       </c>
-      <c r="H3" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="39">
-      <c r="A4" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="G4" s="32">
+      <c r="C5" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="32">
         <v>0.74</v>
       </c>
-      <c r="H4" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="39">
-      <c r="A5" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="E5" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="20"/>
-    </row>
+      <c r="C6" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="18"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="10" spans="1:4" ht="26"/>
+    <row r="11" spans="1:4" ht="26"/>
+    <row r="12" spans="1:4" ht="39"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3785,7 +3720,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>